<commit_message>
added functionality for adding food by employee
</commit_message>
<xml_diff>
--- a/ProjectSchema/projectstatus.xlsx
+++ b/ProjectSchema/projectstatus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Atebal Kant Singh\DjangoWorkspace\canteen\ProjectSchema\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54F4E8DC-6E01-499F-AB88-9A4C63DFE4A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{858B2FEE-DBC0-454E-9852-DEAA3E950804}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4E4F56EB-3265-4FBD-B687-1E96F5D76B47}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="31">
   <si>
     <t xml:space="preserve">Module Name </t>
   </si>
@@ -117,7 +117,7 @@
     <t>checkout--&gt;employee by admin</t>
   </si>
   <si>
-    <t>todo</t>
+    <t xml:space="preserve">in progress need to write function to send isadmin details after clicking on cart button  </t>
   </si>
 </sst>
 </file>
@@ -133,7 +133,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -152,12 +152,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -171,12 +165,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1461,14 +1454,14 @@
   <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="32.21875" customWidth="1"/>
-    <col min="3" max="3" width="16.6640625" customWidth="1"/>
+    <col min="3" max="3" width="72.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1669,6 +1662,9 @@
       <c r="B22" t="s">
         <v>28</v>
       </c>
+      <c r="C22" t="s">
+        <v>5</v>
+      </c>
       <c r="D22" s="1">
         <v>45347</v>
       </c>
@@ -1721,7 +1717,7 @@
       <c r="B27" t="s">
         <v>29</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="C27" s="3" t="s">
         <v>30</v>
       </c>
     </row>

</xml_diff>

<commit_message>
checkout,shopping incart,orders completed for guest
</commit_message>
<xml_diff>
--- a/ProjectSchema/projectstatus.xlsx
+++ b/ProjectSchema/projectstatus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Atebal Kant Singh\DjangoWorkspace\canteen\ProjectSchema\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{858B2FEE-DBC0-454E-9852-DEAA3E950804}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF36D8F7-819B-4211-8B3F-E8EAB98D1E8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4E4F56EB-3265-4FBD-B687-1E96F5D76B47}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="36">
   <si>
     <t xml:space="preserve">Module Name </t>
   </si>
@@ -99,9 +99,6 @@
     <t>delete order--&gt;currentuser</t>
   </si>
   <si>
-    <t>inprogress</t>
-  </si>
-  <si>
     <t>orderplace--&gt;employee by admin</t>
   </si>
   <si>
@@ -117,7 +114,25 @@
     <t>checkout--&gt;employee by admin</t>
   </si>
   <si>
-    <t xml:space="preserve">in progress need to write function to send isadmin details after clicking on cart button  </t>
+    <t>Assign Roles</t>
+  </si>
+  <si>
+    <t>completed</t>
+  </si>
+  <si>
+    <t>Guest Login</t>
+  </si>
+  <si>
+    <t>Payment</t>
+  </si>
+  <si>
+    <t>Menu</t>
+  </si>
+  <si>
+    <t>Update receipe</t>
+  </si>
+  <si>
+    <t>To do</t>
   </si>
 </sst>
 </file>
@@ -133,7 +148,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -143,12 +158,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -165,11 +174,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1142,6 +1150,486 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3970020" y="3779520"/>
+          <a:ext cx="236220" cy="236220"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>701040</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="236220" cy="236220"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Graphic 1" descr="Checkmark">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{86C343CB-7849-49E4-AA4B-3981C2C0E66A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3970020" y="4511040"/>
+          <a:ext cx="236220" cy="236220"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>701040</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="236220" cy="236220"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Graphic 2" descr="Checkmark">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{43DF3EEB-4FFE-46E9-A9B2-1DFD21F3C6F3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3970020" y="4511040"/>
+          <a:ext cx="236220" cy="236220"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>716280</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="236220" cy="236220"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="23" name="Graphic 22" descr="Checkmark">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9B7C47DA-C630-4996-8F76-F5BEE6186593}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3985260" y="3291840"/>
+          <a:ext cx="236220" cy="236220"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>701040</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="236220" cy="236220"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="24" name="Graphic 23" descr="Checkmark">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2FF6CC3A-DE08-41A8-8D4F-CFB8C1216241}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3970020" y="4693920"/>
+          <a:ext cx="236220" cy="236220"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>701040</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="236220" cy="236220"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="25" name="Graphic 24" descr="Checkmark">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{83711973-57D7-49C1-BD98-B816454F913F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3970020" y="4693920"/>
+          <a:ext cx="236220" cy="236220"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>701040</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="236220" cy="236220"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="26" name="Graphic 25" descr="Checkmark">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8CD4C8AA-4F6B-4C93-A685-391614B6D8E6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3970020" y="4876800"/>
+          <a:ext cx="236220" cy="236220"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>701040</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="236220" cy="236220"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="27" name="Graphic 26" descr="Checkmark">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ABC8E02D-3B36-4946-9539-A15A7B64E79F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3970020" y="4876800"/>
+          <a:ext cx="236220" cy="236220"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>701040</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="236220" cy="236220"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="28" name="Graphic 27" descr="Checkmark">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CC6002B3-0F71-4026-B765-4EC0572DDC16}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3970020" y="5059680"/>
+          <a:ext cx="236220" cy="236220"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>701040</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="236220" cy="236220"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="29" name="Graphic 28" descr="Checkmark">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EAACAAAC-E629-445A-BE9D-DB3EC4CD6BA3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3970020" y="5059680"/>
+          <a:ext cx="236220" cy="236220"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>701040</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="236220" cy="236220"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="30" name="Graphic 29" descr="Checkmark">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F32D2B85-5AF8-4A18-8075-E093C3746F17}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3970020" y="5448300"/>
           <a:ext cx="236220" cy="236220"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1451,10 +1939,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E186867D-7D67-4CB9-B552-C0D2AE69C172}">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1632,8 +2120,11 @@
       <c r="B19" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="3" t="s">
-        <v>24</v>
+      <c r="C19" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" s="1">
+        <v>45351</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -1660,7 +2151,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C22" t="s">
         <v>5</v>
@@ -1682,7 +2173,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C24" t="s">
         <v>5</v>
@@ -1693,7 +2184,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C25" t="s">
         <v>5</v>
@@ -1704,7 +2195,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C26" t="s">
         <v>5</v>
@@ -1715,10 +2206,77 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
+        <v>28</v>
+      </c>
+      <c r="C27" t="s">
+        <v>5</v>
+      </c>
+      <c r="D27" s="1">
+        <v>45351</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
         <v>29</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="B28" t="s">
         <v>30</v>
+      </c>
+      <c r="C28" t="s">
+        <v>5</v>
+      </c>
+      <c r="D28" s="1">
+        <v>45351</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29" t="s">
+        <v>30</v>
+      </c>
+      <c r="C29" t="s">
+        <v>5</v>
+      </c>
+      <c r="D29" s="1">
+        <v>45351</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>32</v>
+      </c>
+      <c r="B30" t="s">
+        <v>30</v>
+      </c>
+      <c r="C30" t="s">
+        <v>30</v>
+      </c>
+      <c r="D30" s="1">
+        <v>45351</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>33</v>
+      </c>
+      <c r="B31" t="s">
+        <v>30</v>
+      </c>
+      <c r="C31" t="s">
+        <v>30</v>
+      </c>
+      <c r="D31" s="1">
+        <v>45351</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>34</v>
+      </c>
+      <c r="B32" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add user dashboard,employee orderhistory,payment functionality for employee
</commit_message>
<xml_diff>
--- a/ProjectSchema/projectstatus.xlsx
+++ b/ProjectSchema/projectstatus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Atebal Kant Singh\DjangoWorkspace\canteen\ProjectSchema\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF36D8F7-819B-4211-8B3F-E8EAB98D1E8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90888F40-41AE-4FEA-92A8-778EED658C6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4E4F56EB-3265-4FBD-B687-1E96F5D76B47}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="47">
   <si>
     <t xml:space="preserve">Module Name </t>
   </si>
@@ -133,13 +133,46 @@
   </si>
   <si>
     <t>To do</t>
+  </si>
+  <si>
+    <t>login decorator</t>
+  </si>
+  <si>
+    <t>group_required decorator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Search </t>
+  </si>
+  <si>
+    <t>Payment for Guest user</t>
+  </si>
+  <si>
+    <t>Employee Transactions for Employee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Item of Day list </t>
+  </si>
+  <si>
+    <t>only qunatity can be update</t>
+  </si>
+  <si>
+    <t>creating item of the list</t>
+  </si>
+  <si>
+    <t>Profile</t>
+  </si>
+  <si>
+    <t>in progress</t>
+  </si>
+  <si>
+    <t>Edit Profile</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -147,8 +180,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -161,8 +202,19 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -170,16 +222,35 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Calculation" xfId="1" builtinId="22"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1547,41 +1618,41 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>701040</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>121920</xdr:rowOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="236220" cy="236220"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="29" name="Graphic 28" descr="Checkmark">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EAACAAAC-E629-445A-BE9D-DB3EC4CD6BA3}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
-              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3970020" y="5059680"/>
+        <xdr:cNvPr id="30" name="Graphic 29" descr="Checkmark">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F32D2B85-5AF8-4A18-8075-E093C3746F17}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3970020" y="5448300"/>
           <a:ext cx="236220" cy="236220"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1595,41 +1666,185 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>701040</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>144780</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="236220" cy="236220"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="30" name="Graphic 29" descr="Checkmark">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F32D2B85-5AF8-4A18-8075-E093C3746F17}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
-              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3970020" y="5448300"/>
+        <xdr:cNvPr id="32" name="Graphic 31" descr="Checkmark">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C51C6DBA-569D-4B05-9D52-072683EC591A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4442460" y="5448300"/>
+          <a:ext cx="236220" cy="236220"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>701040</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="236220" cy="236220"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="33" name="Graphic 32" descr="Checkmark">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A3942AB1-D3C2-4C04-96E0-CAAD13AAD7B9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5006340" y="5814060"/>
+          <a:ext cx="236220" cy="236220"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>701040</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="236220" cy="236220"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="34" name="Graphic 33" descr="Checkmark">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00B6BBE9-E426-4498-B974-E517BECF4B4E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5006340" y="5814060"/>
+          <a:ext cx="236220" cy="236220"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>701040</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="236220" cy="236220"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="35" name="Graphic 34" descr="Checkmark">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E39C4918-2E6A-4ABA-A3B4-E9A26BC2C3FA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5006340" y="5814060"/>
           <a:ext cx="236220" cy="236220"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1939,15 +2154,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E186867D-7D67-4CB9-B552-C0D2AE69C172}">
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.5546875" customWidth="1"/>
     <col min="2" max="2" width="32.21875" customWidth="1"/>
     <col min="3" max="3" width="72.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
@@ -2247,15 +2462,10 @@
       <c r="A30" t="s">
         <v>32</v>
       </c>
-      <c r="B30" t="s">
-        <v>30</v>
-      </c>
-      <c r="C30" t="s">
-        <v>30</v>
-      </c>
-      <c r="D30" s="1">
-        <v>45351</v>
-      </c>
+      <c r="B30" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D30" s="1"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
@@ -2275,7 +2485,109 @@
       <c r="A32" t="s">
         <v>34</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D32" s="1">
+        <v>45352</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>36</v>
+      </c>
+      <c r="B33" t="s">
+        <v>30</v>
+      </c>
+      <c r="C33" t="s">
+        <v>30</v>
+      </c>
+      <c r="D33" s="1">
+        <v>45352</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>37</v>
+      </c>
+      <c r="B34" t="s">
+        <v>30</v>
+      </c>
+      <c r="C34" t="s">
+        <v>30</v>
+      </c>
+      <c r="D34" s="1">
+        <v>45352</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>38</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>39</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>40</v>
+      </c>
+      <c r="B37" t="s">
+        <v>30</v>
+      </c>
+      <c r="C37" t="s">
+        <v>30</v>
+      </c>
+      <c r="D37" s="1">
+        <v>45352</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>41</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>43</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>44</v>
+      </c>
+      <c r="B40" t="s">
+        <v>30</v>
+      </c>
+      <c r="C40" t="s">
+        <v>30</v>
+      </c>
+      <c r="D40" s="1">
+        <v>45352</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>46</v>
+      </c>
+      <c r="B41" s="3" t="s">
         <v>35</v>
       </c>
     </row>

</xml_diff>

<commit_message>
CRUD for receipe and item of the day
</commit_message>
<xml_diff>
--- a/ProjectSchema/projectstatus.xlsx
+++ b/ProjectSchema/projectstatus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Atebal Kant Singh\DjangoWorkspace\canteen\ProjectSchema\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9A5CBF6-7D99-453F-B919-ABA654F10069}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5E4F6FA-839F-4DD8-A032-E31D4075BF89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4E4F56EB-3265-4FBD-B687-1E96F5D76B47}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="48">
   <si>
     <t xml:space="preserve">Module Name </t>
   </si>
@@ -153,22 +153,22 @@
     <t xml:space="preserve">Item of Day list </t>
   </si>
   <si>
-    <t>only qunatity can be update</t>
-  </si>
-  <si>
     <t>creating item of the list</t>
   </si>
   <si>
     <t>Profile</t>
   </si>
   <si>
-    <t>in progress</t>
-  </si>
-  <si>
     <t>Edit Profile</t>
   </si>
   <si>
     <t>complete Except update Address</t>
+  </si>
+  <si>
+    <t>Add Receipe</t>
+  </si>
+  <si>
+    <t>in progress incorporate payment</t>
   </si>
 </sst>
 </file>
@@ -1573,41 +1573,41 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>701040</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>121920</xdr:rowOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="236220" cy="236220"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="28" name="Graphic 27" descr="Checkmark">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CC6002B3-0F71-4026-B765-4EC0572DDC16}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
-              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3970020" y="5059680"/>
+        <xdr:cNvPr id="30" name="Graphic 29" descr="Checkmark">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F32D2B85-5AF8-4A18-8075-E093C3746F17}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3970020" y="5448300"/>
           <a:ext cx="236220" cy="236220"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1621,41 +1621,41 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>701040</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>144780</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="236220" cy="236220"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="30" name="Graphic 29" descr="Checkmark">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F32D2B85-5AF8-4A18-8075-E093C3746F17}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
-              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3970020" y="5448300"/>
+        <xdr:cNvPr id="32" name="Graphic 31" descr="Checkmark">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C51C6DBA-569D-4B05-9D52-072683EC591A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4442460" y="5448300"/>
           <a:ext cx="236220" cy="236220"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1675,35 +1675,35 @@
     <xdr:ext cx="236220" cy="236220"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="32" name="Graphic 31" descr="Checkmark">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C51C6DBA-569D-4B05-9D52-072683EC591A}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
-              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4442460" y="5448300"/>
+        <xdr:cNvPr id="33" name="Graphic 32" descr="Checkmark">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A3942AB1-D3C2-4C04-96E0-CAAD13AAD7B9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5006340" y="5814060"/>
           <a:ext cx="236220" cy="236220"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1717,16 +1717,16 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>701040</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>144780</xdr:rowOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="236220" cy="236220"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="33" name="Graphic 32" descr="Checkmark">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A3942AB1-D3C2-4C04-96E0-CAAD13AAD7B9}"/>
+        <xdr:cNvPr id="34" name="Graphic 33" descr="Checkmark">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00B6BBE9-E426-4498-B974-E517BECF4B4E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1771,10 +1771,10 @@
     <xdr:ext cx="236220" cy="236220"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="34" name="Graphic 33" descr="Checkmark">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00B6BBE9-E426-4498-B974-E517BECF4B4E}"/>
+        <xdr:cNvPr id="35" name="Graphic 34" descr="Checkmark">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E39C4918-2E6A-4ABA-A3B4-E9A26BC2C3FA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1813,41 +1813,185 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>701040</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>144780</xdr:rowOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="236220" cy="236220"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="35" name="Graphic 34" descr="Checkmark">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E39C4918-2E6A-4ABA-A3B4-E9A26BC2C3FA}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
-              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5006340" y="5814060"/>
+        <xdr:cNvPr id="29" name="Graphic 28" descr="Checkmark">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{248C182D-9B3B-4CCE-8A59-C49E8435564A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5006340" y="6713220"/>
+          <a:ext cx="236220" cy="236220"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>662940</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="236220" cy="236220"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="31" name="Graphic 30" descr="Checkmark">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{62C31068-02EA-4598-91BC-721DB3CB2642}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4968240" y="6172200"/>
+          <a:ext cx="236220" cy="236220"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>662940</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="236220" cy="236220"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="36" name="Graphic 35" descr="Checkmark">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{003D05FD-D34B-4895-BC4E-D32F8EC8C493}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4968240" y="6385560"/>
+          <a:ext cx="236220" cy="236220"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>701040</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="236220" cy="236220"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="37" name="Graphic 36" descr="Checkmark">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B1F3FC2F-024C-4281-A518-77337639BBED}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5006340" y="5303520"/>
           <a:ext cx="236220" cy="236220"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2157,10 +2301,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E186867D-7D67-4CB9-B552-C0D2AE69C172}">
-  <dimension ref="A1:D41"/>
+  <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2463,33 +2607,41 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>32</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D30" s="1"/>
+        <v>33</v>
+      </c>
+      <c r="B30" t="s">
+        <v>30</v>
+      </c>
+      <c r="C30" t="s">
+        <v>30</v>
+      </c>
+      <c r="D30" s="1">
+        <v>45351</v>
+      </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B31" t="s">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="C31" t="s">
         <v>30</v>
       </c>
       <c r="D31" s="1">
-        <v>45351</v>
+        <v>45358</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>34</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
+      </c>
+      <c r="B32" t="s">
+        <v>30</v>
+      </c>
+      <c r="C32" t="s">
+        <v>30</v>
       </c>
       <c r="D32" s="1">
         <v>45352</v>
@@ -2497,7 +2649,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B33" t="s">
         <v>30</v>
@@ -2511,7 +2663,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B34" t="s">
         <v>30</v>
@@ -2525,23 +2677,35 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>38</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>35</v>
+        <v>41</v>
+      </c>
+      <c r="B35" t="s">
+        <v>5</v>
+      </c>
+      <c r="C35" t="s">
+        <v>5</v>
+      </c>
+      <c r="D35" s="1">
+        <v>45358</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>39</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>45</v>
+        <v>42</v>
+      </c>
+      <c r="B36" t="s">
+        <v>5</v>
+      </c>
+      <c r="C36" t="s">
+        <v>5</v>
+      </c>
+      <c r="D36" s="1">
+        <v>45358</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B37" t="s">
         <v>30</v>
@@ -2555,18 +2719,21 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>41</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>35</v>
+        <v>46</v>
+      </c>
+      <c r="B38" t="s">
+        <v>30</v>
+      </c>
+      <c r="C38" t="s">
+        <v>30</v>
+      </c>
+      <c r="D38" s="1">
+        <v>45358</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>35</v>
@@ -2576,21 +2743,24 @@
       <c r="A40" t="s">
         <v>44</v>
       </c>
-      <c r="B40" t="s">
-        <v>30</v>
-      </c>
-      <c r="C40" t="s">
-        <v>30</v>
-      </c>
-      <c r="D40" s="1">
-        <v>45352</v>
+      <c r="B40" s="3" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>46</v>
-      </c>
-      <c r="B41" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D41" s="1"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>39</v>
+      </c>
+      <c r="B42" s="4" t="s">
         <v>47</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add user by admin,add address and edit address, payment by admin and admin can recharge for user
</commit_message>
<xml_diff>
--- a/ProjectSchema/projectstatus.xlsx
+++ b/ProjectSchema/projectstatus.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Atebal Kant Singh\DjangoWorkspace\canteen\ProjectSchema\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5E4F6FA-839F-4DD8-A032-E31D4075BF89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B78AFF4-1A27-43BE-A645-E3408FFD98B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4E4F56EB-3265-4FBD-B687-1E96F5D76B47}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="46">
   <si>
     <t xml:space="preserve">Module Name </t>
   </si>
@@ -132,9 +132,6 @@
     <t>Update receipe</t>
   </si>
   <si>
-    <t>To do</t>
-  </si>
-  <si>
     <t>login decorator</t>
   </si>
   <si>
@@ -162,20 +159,17 @@
     <t>Edit Profile</t>
   </si>
   <si>
-    <t>complete Except update Address</t>
-  </si>
-  <si>
     <t>Add Receipe</t>
   </si>
   <si>
-    <t>in progress incorporate payment</t>
+    <t>Add user by Admin</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -183,16 +177,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="5">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -205,19 +191,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -225,35 +200,16 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Calculation" xfId="1" builtinId="22"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1992,6 +1948,246 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5006340" y="5303520"/>
+          <a:ext cx="236220" cy="236220"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>701040</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="236220" cy="236220"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="28" name="Graphic 27" descr="Checkmark">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{49A996D5-8D62-443B-9AC4-B7F9017CCD80}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5006340" y="6713220"/>
+          <a:ext cx="236220" cy="236220"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>701040</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="236220" cy="236220"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="38" name="Graphic 37" descr="Checkmark">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DE63FDBF-CED9-4F52-A9EF-877090641E9F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5006340" y="6896100"/>
+          <a:ext cx="236220" cy="236220"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>701040</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="236220" cy="236220"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="39" name="Graphic 38" descr="Checkmark">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{39217C2F-9EA0-46BA-B134-9534F0AC5FA4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5006340" y="6896100"/>
+          <a:ext cx="236220" cy="236220"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>701040</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="236220" cy="236220"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="40" name="Graphic 39" descr="Checkmark">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{78892A9D-842D-408E-99F4-24C67D337DB4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5006340" y="6896100"/>
+          <a:ext cx="236220" cy="236220"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>701040</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="236220" cy="236220"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="41" name="Graphic 40" descr="Checkmark">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EC8D545B-312F-4AB5-B967-533EE6464A8F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5006340" y="6896100"/>
           <a:ext cx="236220" cy="236220"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2301,10 +2497,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E186867D-7D67-4CB9-B552-C0D2AE69C172}">
-  <dimension ref="A1:D42"/>
+  <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2635,7 +2831,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B32" t="s">
         <v>30</v>
@@ -2649,7 +2845,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B33" t="s">
         <v>30</v>
@@ -2663,7 +2859,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B34" t="s">
         <v>30</v>
@@ -2677,7 +2873,7 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B35" t="s">
         <v>5</v>
@@ -2691,7 +2887,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B36" t="s">
         <v>5</v>
@@ -2705,7 +2901,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B37" t="s">
         <v>30</v>
@@ -2719,7 +2915,7 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B38" t="s">
         <v>30</v>
@@ -2733,35 +2929,72 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>38</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>35</v>
+        <v>37</v>
+      </c>
+      <c r="B39" t="s">
+        <v>30</v>
+      </c>
+      <c r="C39" t="s">
+        <v>30</v>
+      </c>
+      <c r="D39" s="1">
+        <v>45359</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>44</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
+      </c>
+      <c r="B40" t="s">
+        <v>30</v>
+      </c>
+      <c r="C40" t="s">
+        <v>30</v>
+      </c>
+      <c r="D40" s="1">
+        <v>45359</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>32</v>
       </c>
-      <c r="B41" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="D41" s="1"/>
+      <c r="B41" t="s">
+        <v>30</v>
+      </c>
+      <c r="C41" t="s">
+        <v>30</v>
+      </c>
+      <c r="D41" s="1">
+        <v>45359</v>
+      </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>39</v>
-      </c>
-      <c r="B42" s="4" t="s">
-        <v>47</v>
+        <v>38</v>
+      </c>
+      <c r="B42" t="s">
+        <v>30</v>
+      </c>
+      <c r="C42" t="s">
+        <v>30</v>
+      </c>
+      <c r="D42" s="1">
+        <v>45359</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>45</v>
+      </c>
+      <c r="B43" t="s">
+        <v>5</v>
+      </c>
+      <c r="C43" t="s">
+        <v>30</v>
+      </c>
+      <c r="D43" s="1">
+        <v>45359</v>
       </c>
     </row>
   </sheetData>

</xml_diff>